<commit_message>
update cebu test e2e
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Thaiairways\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Cebu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F090D970-FFED-4E01-A4EE-9F4DB1BB0356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C121FB-0EF8-41FC-8769-DBB678315E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -217,13 +217,13 @@
     <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
   </si>
   <si>
-    <t>RPA206_ThaiAirways_RefID</t>
-  </si>
-  <si>
-    <t>RefId</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>RPAXXX_Cebu_Domain</t>
+  </si>
+  <si>
+    <t>Domain</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -1693,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2857,9 +2857,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2965,10 +2965,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3958,7 +3958,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update cebu converter & validation
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Cebu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C121FB-0EF8-41FC-8769-DBB678315E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFFFBA2-58D8-431F-AB23-80DF9C37B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -220,10 +220,37 @@
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>RPAXXX_Cebu_Domain</t>
-  </si>
-  <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>PathMailValidation</t>
+  </si>
+  <si>
+    <t>PathValidation</t>
+  </si>
+  <si>
+    <t>Validation SOA  vs Payment Receipt</t>
+  </si>
+  <si>
+    <t>Data\EmailTemplate\Cebu_Validation.html</t>
+  </si>
+  <si>
+    <t>Data\Temp\Validation.txt</t>
+  </si>
+  <si>
+    <t>MailValidationTo</t>
+  </si>
+  <si>
+    <t>MailValidationCc</t>
+  </si>
+  <si>
+    <t>RPA234_Cebu_Domain</t>
+  </si>
+  <si>
+    <t>RPA234_Cebu_MailValidationTo</t>
+  </si>
+  <si>
+    <t>RPA234_Cebu_MailValidationCc</t>
   </si>
 </sst>
 </file>
@@ -602,16 +629,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1"/>
-    <col min="2" max="2" width="62.21875" customWidth="1"/>
-    <col min="3" max="3" width="81.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="3" max="3" width="81.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -659,7 +686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -669,7 +696,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -691,8 +718,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1697,12 +1744,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1739,7 +1786,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1864,7 +1911,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2859,16 +2906,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="42.77734375" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2965,14 +3012,28 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
update cebu e2e pre SIT
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Cebu/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Cebu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFFFBA2-58D8-431F-AB23-80DF9C37B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428131AF-7B2C-48BD-9F55-67BC378E3A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -251,6 +251,15 @@
   </si>
   <si>
     <t>RPA234_Cebu_MailValidationCc</t>
+  </si>
+  <si>
+    <t>PathTemplatePaymentReceipt</t>
+  </si>
+  <si>
+    <t>Data\Template\Template-PaymentReceipt.xlsx</t>
+  </si>
+  <si>
+    <t>Template Report Payment Receipt</t>
   </si>
 </sst>
 </file>
@@ -630,15 +639,15 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="81.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="81.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -686,7 +695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -696,7 +705,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -740,7 +749,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1744,12 +1763,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1786,7 +1805,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1797,7 +1816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1911,7 +1930,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2910,12 +2929,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>